<commit_message>
Generalizing scripts to any project
While summarizing RunMS51, I'm working to make scripts more useful for future data sets and projects. Changes include:

- R/functions/summarize.depth.at.target.SNPs.R is now a function rather than a script. The script R/BAM.SAM.handling/depth at .target.SNPs.R shows how to use it for a specific set of data.
- R/BAM.SAM.handling.R is a script that combines the utility of R/fastq.handling/Start here Summarize.fastq.files.R and depth.at.target.SNPs.R into a single place. It's easily customizable for any set of data, though it does assume you've already used samtools to calculate read depth at target loci.
- I've added a function in R/functions/compare.replicates.R to compare genotypes across replicate samples to look for mismatches. The script R/call.genos/RunMS51.compare.replicates.R demonstrates its use for a specific set of data

Other changes are specific to my new data set.
</commit_message>
<xml_diff>
--- a/results-raw/Primers mapped to genome summary.xlsx
+++ b/results-raw/Primers mapped to genome summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/KKMDocuments/Documents/Github.Repos/Mnov/GTseq.design.and.QAQC/results-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2B1D07-E1A8-864B-9522-057767BD5377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEF9B71-413A-3D40-A2D9-D66B4563E0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15600" yWindow="10640" windowWidth="27240" windowHeight="16440" xr2:uid="{5FDF951B-6050-6F4A-A029-C7401EA8BF2A}"/>
   </bookViews>
@@ -5803,10 +5803,13 @@
   <dimension ref="A1:W1057"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>